<commit_message>
This is latest code for new tc
</commit_message>
<xml_diff>
--- a/src/test/resources/input_data.xlsx
+++ b/src/test/resources/input_data.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharatkammakatla/TestAutomation/SeleniumJavaFramework/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SDE47\eclipse-workspace\Selenium-Java-Framework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49FCA8B3-22CB-F049-9291-C9AD4737F083}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2463F9C5-1750-0048-8FEB-74FF33B32275}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -63,19 +62,19 @@
     <t>TC3</t>
   </si>
   <si>
-    <t>CURA Healthcare</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>CURA Healthcare Service</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -448,33 +447,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{745E163B-7AA0-DE48-B629-E9896DDF2F3D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
@@ -489,7 +488,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -500,7 +499,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -520,12 +519,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>